<commit_message>
Première base du fichier html
</commit_message>
<xml_diff>
--- a/Tableaux/recap_SOM.xlsx
+++ b/Tableaux/recap_SOM.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">ID_Neurone</t>
   </si>
@@ -20,76 +20,70 @@
     <t xml:space="preserve">Joueurs</t>
   </si>
   <si>
-    <t xml:space="preserve">Thib_S5, Grenzo, Corentin, Jilink, Chopa, Cha, Alan_S9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bilel_S4, Bylost_S4, And, Xiao, Nikolas_S5, Gririsu_S5, Nath_S6, Clovis, Cosmos, Piiskoo, Z4tix_S9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Line, Julien_S5, Timeo_S5, Black Lolo_S5, Amaury_S5, Kwinn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyrf, Sneus, Ethan_S3, Malkovan_S3, Bylost, HiYoucef</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flau, Nath, Ranzyo, Guigui, Angel, Mtking, Dragon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saucisson, Ranzyo_S5, Killian, Waikato, Mickey, Pilouche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nelson_S4, Alex., Raphi, Xiao_S5, Gwendal_S7, Enze_S7, Thynael</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skowa_S4, Saucisson_S5, Malkovan_S5, Manta, Dahmi1 Arti, Gobou_S6, Lilian, Mehdiiii, Quentin, Alex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crypto, Yatho, Vah Balress, Mistimat, Guigui_S9</t>
+    <t xml:space="preserve">Saucisson, Ranzyo_S5, Thib_S5, Grenzo, Jilink, Chopa, Cha, Alan_S9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The soulless, Killian, Julien_S7, Waikato, Mickey, Pilouche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chreet, Joshua, Gririsu, Hugo, Thib, Julien, Mickey_S8, Sunka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alecxperdu, Nelson, DTP, DramaPanda, Maitredoudou, FooD_Flo, Chreet_S5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nikolas, Gwendal, Clem fair play, Timeo, Amaury, Malkovan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bilel_S4, Bylost_S4, And, Xiao, Clovis, Thynael, Cosmos, Z4tix_S9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nelson_S4, Alex., Skowa_S4, Raphi, Xiao_S5, Manta, Dahmi1 Arti, Gobou_S6, Gwendal_S7, Lilian, Mehdiiii, Corentin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Lolo, FooD_Flo_S5, Enze, Doggydog_S6, Enze_S7, Tim, Luc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamiga, Z4tix, Mark, Alecxperdu_S2, Gobou, Polo, Skowa, Mark_S2, Schweppes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bylost, Nikolas_S5, Gririsu_S5, Nath_S6, Piiskoo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes_S6, Ethan_S6, Gigi, Quentin, Enze_S8, Alex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eneko, Xori, Thyx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethan, Nicovid, Ladoly, Didine, Deku, Sayo, Line_S5, Clem fair play_S5, TimeoGnc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyrf, Sneus, Malkovan_S3, Julien_S5, Timeo_S5, Black Lolo_S5, Amaury_S5, Kwinn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line, HiYoucef, Saucisson_S5, Malkovan_S5, Vah Balress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crypto, Yatho, Mistimat, Spider, Guigui_S9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yuu, Nounours, Saminette, Nicovid_S6, Cyrf_S6, Blacks Star, Kamiga_S9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krak, Nwog, Jehovah, Alexadventure, Step, Feiik, Tiff, Natoxe, Bilal, Flau_S4, Bilel_S5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flau, Nath, Ethan_S3, Ranzyo, Guigui, Angel, Mtking, Dragon</t>
   </si>
   <si>
     <t xml:space="preserve">Bilel, Joshua_S3, GiulfeuYT, Doggydog, Alan, Mark_S5, Maitredoudou_S5</t>
   </si>
   <si>
-    <t xml:space="preserve">The soulless, Julien_S7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black Lolo, Eneko, FooD_Flo_S5, Enze, Thyx, Doggydog_S6, Tim, Luc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppes_S6, Ethan_S6, Xori, Gigi, Spider, Enze_S8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kamiga_S5, GiulfeuYT_S6, Alan_S7, Sy_boulette, Reiko, Ju, Mielle</t>
   </si>
   <si>
-    <t xml:space="preserve">Yuu, Nounours, Saminette, Nicovid_S6, Cyrf_S6, Blacks Star, Kamiga_S9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chreet, Thib, Julien, Mickey_S8, Sunka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chreet_S5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kamiga, Z4tix, Mark, Gwendal, Alecxperdu_S2, Gobou, Polo, Clem fair play, Skowa, Mark_S2, Timeo, Amaury, Schweppes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Line_S5, Clem fair play_S5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Blgham</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nikolas, Joshua, Gririsu, Hugo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alecxperdu, Nelson, DTP, DramaPanda, Maitredoudou, FooD_Flo, Malkovan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jehovah, Nicovid, Ladoly, Deku, Sayo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Krak, Nwog, Ethan, Alexadventure, Step, Feiik, Tiff, Natoxe, Bilal, Flau_S4, Didine, Bilel_S5, TimeoGnc</t>
   </si>
   <si>
     <t xml:space="preserve">Lili, Samson, SorciShoot, Louan, Xo, Napoleon, Cyrf_S4, Espoir Perdu, And_S5, Major Chris, Nikolas_S6, Nemocca, Aurel, Theo, Chatoon, Clement, Mizuki, Armand, Manu</t>
@@ -498,7 +492,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -506,7 +500,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -514,7 +508,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -522,7 +516,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -530,7 +524,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -538,7 +532,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -546,7 +540,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -554,7 +548,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -562,7 +556,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -570,7 +564,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -578,7 +572,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -586,7 +580,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
@@ -594,7 +588,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
@@ -602,7 +596,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
@@ -610,26 +604,10 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version finale du html
</commit_message>
<xml_diff>
--- a/Tableaux/recap_SOM.xlsx
+++ b/Tableaux/recap_SOM.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">ID_Neurone</t>
   </si>
@@ -20,73 +20,79 @@
     <t xml:space="preserve">Joueurs</t>
   </si>
   <si>
-    <t xml:space="preserve">Saucisson, Ranzyo_S5, Thib_S5, Grenzo, Jilink, Chopa, Cha, Alan_S9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The soulless, Killian, Julien_S7, Waikato, Mickey, Pilouche</t>
+    <t xml:space="preserve">Nikolas, Timeo, Malkovan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alecxperdu, Nelson, DTP, DramaPanda, Maitredoudou, FooD_Flo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alecxperdu_S2, Gobou, Polo, Skowa, Mark_S2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krak, Nwog, Ethan, Jehovah, Alexadventure, Step, Feiik, Tiff, Natoxe, Bilal, Flau_S4, Didine, Bilel_S5, TimeoGnc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lili, Samson, SorciShoot, Louan, Xo, Napoleon, Cyrf_S4, Espoir Perdu, And_S5, Major Chris, Nikolas_S6, Nemocca, Aurel, Theo, Chatoon, Clement, Mizuki, Armand, Manu</t>
   </si>
   <si>
     <t xml:space="preserve">Chreet, Joshua, Gririsu, Hugo, Thib, Julien, Mickey_S8, Sunka</t>
   </si>
   <si>
-    <t xml:space="preserve">Alecxperdu, Nelson, DTP, DramaPanda, Maitredoudou, FooD_Flo, Chreet_S5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nikolas, Gwendal, Clem fair play, Timeo, Amaury, Malkovan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bilel_S4, Bylost_S4, And, Xiao, Clovis, Thynael, Cosmos, Z4tix_S9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nelson_S4, Alex., Skowa_S4, Raphi, Xiao_S5, Manta, Dahmi1 Arti, Gobou_S6, Gwendal_S7, Lilian, Mehdiiii, Corentin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black Lolo, FooD_Flo_S5, Enze, Doggydog_S6, Enze_S7, Tim, Luc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kamiga, Z4tix, Mark, Alecxperdu_S2, Gobou, Polo, Skowa, Mark_S2, Schweppes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bylost, Nikolas_S5, Gririsu_S5, Nath_S6, Piiskoo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppes_S6, Ethan_S6, Gigi, Quentin, Enze_S8, Alex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eneko, Xori, Thyx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ethan, Nicovid, Ladoly, Didine, Deku, Sayo, Line_S5, Clem fair play_S5, TimeoGnc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyrf, Sneus, Malkovan_S3, Julien_S5, Timeo_S5, Black Lolo_S5, Amaury_S5, Kwinn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Line, HiYoucef, Saucisson_S5, Malkovan_S5, Vah Balress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crypto, Yatho, Mistimat, Spider, Guigui_S9</t>
+    <t xml:space="preserve">Chreet_S5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamiga, Z4tix, Mark, Gwendal, Clem fair play, Amaury, Schweppes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicovid, Ladoly, Deku, Sayo, Line_S5, Clem fair play_S5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blgham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The soulless, FooD_Flo_S5, Julien_S7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Lolo, Eneko, Enze, Thyx, Doggydog_S6, Tim, Luc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes_S6, Ethan_S6, Xori, Gigi, Spider, Enze_S8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamiga_S5, GiulfeuYT_S6, Alan_S7, Sy_boulette, Reiko, Ju, Mielle</t>
   </si>
   <si>
     <t xml:space="preserve">Yuu, Nounours, Saminette, Nicovid_S6, Cyrf_S6, Blacks Star, Kamiga_S9</t>
   </si>
   <si>
-    <t xml:space="preserve">Krak, Nwog, Jehovah, Alexadventure, Step, Feiik, Tiff, Natoxe, Bilal, Flau_S4, Bilel_S5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flau, Nath, Ethan_S3, Ranzyo, Guigui, Angel, Mtking, Dragon</t>
+    <t xml:space="preserve">Saucisson, Ranzyo_S5, Killian, Waikato, Mickey, Jilink, Pilouche, Alan_S9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nelson_S4, Alex., Skowa_S4, Raphi, Xiao_S5, Manta, Dahmi1 Arti, Gobou_S6, Gwendal_S7, Enze_S7, Lilian, Mehdiiii, Corentin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bylost, Line, HiYoucef, Saucisson_S5, Malkovan_S5, Quentin, Alex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crypto, Yatho, Vah Balress, Mistimat, Guigui_S9, Mtking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bilel_S4, Bylost_S4, Thib_S5, Grenzo, Chopa, Cha, Z4tix_S9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">And, Xiao, Gririsu_S5, Nath_S6, Clovis, Thynael, Cosmos, Piiskoo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyrf, Sneus, Malkovan_S3, Julien_S5, Timeo_S5, Black Lolo_S5, Nikolas_S5, Amaury_S5, Kwinn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nath, Ethan_S3, Ranzyo, Guigui, Angel, Dragon</t>
   </si>
   <si>
     <t xml:space="preserve">Bilel, Joshua_S3, GiulfeuYT, Doggydog, Alan, Mark_S5, Maitredoudou_S5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kamiga_S5, GiulfeuYT_S6, Alan_S7, Sy_boulette, Reiko, Ju, Mielle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blgham</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lili, Samson, SorciShoot, Louan, Xo, Napoleon, Cyrf_S4, Espoir Perdu, And_S5, Major Chris, Nikolas_S6, Nemocca, Aurel, Theo, Chatoon, Clement, Mizuki, Armand, Manu</t>
   </si>
 </sst>
 </file>
@@ -492,7 +498,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -500,7 +506,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -508,7 +514,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -516,7 +522,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -524,7 +530,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -532,7 +538,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -540,7 +546,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -548,7 +554,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -556,7 +562,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -564,7 +570,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -572,7 +578,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -580,7 +586,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
@@ -588,7 +594,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
@@ -596,7 +602,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
@@ -604,10 +610,26 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modification du script R size
</commit_message>
<xml_diff>
--- a/Tableaux/recap_SOM.xlsx
+++ b/Tableaux/recap_SOM.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">ID_Neurone</t>
   </si>
@@ -20,79 +20,52 @@
     <t xml:space="preserve">Joueurs</t>
   </si>
   <si>
-    <t xml:space="preserve">Nikolas, Timeo, Malkovan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alecxperdu, Nelson, DTP, DramaPanda, Maitredoudou, FooD_Flo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alecxperdu_S2, Gobou, Polo, Skowa, Mark_S2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Krak, Nwog, Ethan, Jehovah, Alexadventure, Step, Feiik, Tiff, Natoxe, Bilal, Flau_S4, Didine, Bilel_S5, TimeoGnc</t>
+    <t xml:space="preserve">Alecxperdu, DTP, DramaPanda, Maitredoudou, FooD_Flo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chreet, Joshua, Gririsu, Hugo, Thib, Julien, Chreet_S5, Mickey_S8, Sunka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saucisson, The soulless, Ranzyo_S5, Killian, Gwendal_S7, Julien_S7, Waikato, Mickey, Pilouche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bilel_S4, Bylost_S4, And, Xiao, Nikolas_S5, Gririsu_S5, Thib_S5, Nath_S6, Grenzo, Clovis, Thynael, Cosmos, Piiskoo, Chopa, Cha, Z4tix_S9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamiga, Nelson, Mark, Alecxperdu_S2, Gobou, Polo, Skowa, Mark_S2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z4tix, Nikolas, Gwendal, Clem fair play, Timeo, Amaury, Schweppes, Malkovan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Lolo, Eneko, FooD_Flo_S5, Enze, Thyx, Doggydog_S6, Enze_S7, Tim, Luc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nelson_S4, Alex., Skowa_S4, Raphi, Xiao_S5, Manta, Dahmi1 Arti, Gobou_S6, Lilian, Mehdiiii, Corentin, Jilink, Alan_S9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krak, Nwog, Ethan, Jehovah, Nicovid, Alexadventure, Step, Feiik, Tiff, Ladoly, Natoxe, Bilal, Flau_S4, Didine, Deku, Sayo, Line_S5, Bilel_S5, Clem fair play_S5, TimeoGnc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamiga_S5, GiulfeuYT_S6, Alan_S7, Sy_boulette, Reiko, Ju, Mielle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saucisson_S5, Malkovan_S5, Schweppes_S6, Ethan_S6, Xori, Crypto, Yatho, Vah Balress, Gigi, Quentin, Mistimat, Spider, Enze_S8, Alex, Guigui_S9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyrf, Sneus, Malkovan_S3, Bylost, Line, HiYoucef, Julien_S5, Timeo_S5, Black Lolo_S5, Amaury_S5, Kwinn</t>
   </si>
   <si>
     <t xml:space="preserve">Lili, Samson, SorciShoot, Louan, Xo, Napoleon, Cyrf_S4, Espoir Perdu, And_S5, Major Chris, Nikolas_S6, Nemocca, Aurel, Theo, Chatoon, Clement, Mizuki, Armand, Manu</t>
   </si>
   <si>
-    <t xml:space="preserve">Chreet, Joshua, Gririsu, Hugo, Thib, Julien, Mickey_S8, Sunka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chreet_S5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kamiga, Z4tix, Mark, Gwendal, Clem fair play, Amaury, Schweppes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicovid, Ladoly, Deku, Sayo, Line_S5, Clem fair play_S5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blgham</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The soulless, FooD_Flo_S5, Julien_S7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black Lolo, Eneko, Enze, Thyx, Doggydog_S6, Tim, Luc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppes_S6, Ethan_S6, Xori, Gigi, Spider, Enze_S8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kamiga_S5, GiulfeuYT_S6, Alan_S7, Sy_boulette, Reiko, Ju, Mielle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yuu, Nounours, Saminette, Nicovid_S6, Cyrf_S6, Blacks Star, Kamiga_S9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saucisson, Ranzyo_S5, Killian, Waikato, Mickey, Jilink, Pilouche, Alan_S9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nelson_S4, Alex., Skowa_S4, Raphi, Xiao_S5, Manta, Dahmi1 Arti, Gobou_S6, Gwendal_S7, Enze_S7, Lilian, Mehdiiii, Corentin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bylost, Line, HiYoucef, Saucisson_S5, Malkovan_S5, Quentin, Alex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crypto, Yatho, Vah Balress, Mistimat, Guigui_S9, Mtking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bilel_S4, Bylost_S4, Thib_S5, Grenzo, Chopa, Cha, Z4tix_S9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">And, Xiao, Gririsu_S5, Nath_S6, Clovis, Thynael, Cosmos, Piiskoo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyrf, Sneus, Malkovan_S3, Julien_S5, Timeo_S5, Black Lolo_S5, Nikolas_S5, Amaury_S5, Kwinn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nath, Ethan_S3, Ranzyo, Guigui, Angel, Dragon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bilel, Joshua_S3, GiulfeuYT, Doggydog, Alan, Mark_S5, Maitredoudou_S5</t>
+    <t xml:space="preserve">Yuu, Nounours, Saminette, Cyrf_S6, Blgham, Blacks Star, Kamiga_S9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bilel, Joshua_S3, GiulfeuYT, Doggydog, Alan, Mark_S5, Maitredoudou_S5, Nicovid_S6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flau, Nath, Ethan_S3, Ranzyo, Guigui, Angel, Mtking, Dragon</t>
   </si>
 </sst>
 </file>
@@ -560,78 +533,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>